<commit_message>
Update dashboard data - New Excel file uploaded
📊 Data Update Summary:
- Audit Count records: 157 (was 150) - +7 records
- Recruiter Wise Data records: 597 (was 567) - +30 records
- JSON file size: 303 KB (was 288 KB)
- Excel file size: 50 KB (was 48 KB)

Changes:
- Updated 'Power BI Dashboard Data.xlsx' with latest data
- Regenerated 'sample-data.json' with new records
- Dashboard will auto-load updated data on page load

Sheet Names (with trailing spaces):
- 'Audit Count ' (15 columns)
- 'Recruiter Wise Data ' (10 columns)

Data is now live and ready to view!
</commit_message>
<xml_diff>
--- a/Power BI Dashboard Data.xlsx
+++ b/Power BI Dashboard Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://peoplestronghrservices-my.sharepoint.com/personal/rishab_jha_taggd_in/Documents/Desktop/Adani Cements/Jul'25/Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1178" documentId="8_{F1BBBB7F-47AE-4CE6-A18B-5A5C84E2A5BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10123C43-9711-4FF0-A3A6-69F990E7A00C}"/>
+  <xr:revisionPtr revIDLastSave="1242" documentId="8_{F1BBBB7F-47AE-4CE6-A18B-5A5C84E2A5BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5CEFF3A-519B-4E90-AE16-A60209A212D0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{209BDCAE-15BA-4B15-8BF8-E4A28D2CEB45}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Audit Count '!$A$1:$O$134</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Recruiter Wise Data '!$A$1:$J$568</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Recruiter Wise Data '!$A$1:$J$598</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4795" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5052" uniqueCount="88">
   <si>
     <t>Client</t>
   </si>
@@ -400,7 +400,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -433,9 +433,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7272780-F6E8-4A36-B6CD-CC205CD51139}">
-  <dimension ref="A1:P151"/>
+  <dimension ref="A1:P158"/>
   <sheetViews>
-    <sheetView topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="G151" sqref="G151"/>
+    <sheetView topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="G158" sqref="G158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7532,7 +7529,7 @@
         <v>0</v>
       </c>
       <c r="M135" s="10">
-        <f t="shared" ref="M135:M141" si="43">J135/(I135-L135)</f>
+        <f t="shared" ref="M135:M158" si="43">J135/(I135-L135)</f>
         <v>1</v>
       </c>
       <c r="N135" s="10">
@@ -7882,15 +7879,15 @@
         <v>5</v>
       </c>
       <c r="M142" s="10">
-        <f t="shared" ref="M142:M144" si="46">J142/(I142-L142)</f>
+        <f t="shared" si="43"/>
         <v>1</v>
       </c>
       <c r="N142" s="10">
-        <f t="shared" ref="N142:N144" si="47">K142/(I142-L142)</f>
+        <f t="shared" ref="N142:N144" si="46">K142/(I142-L142)</f>
         <v>0</v>
       </c>
       <c r="O142" s="10">
-        <f t="shared" ref="O142:O144" si="48">I142/H142</f>
+        <f t="shared" ref="O142:O144" si="47">I142/H142</f>
         <v>0.5</v>
       </c>
     </row>
@@ -7932,15 +7929,15 @@
         <v>3</v>
       </c>
       <c r="M143" s="10">
+        <f t="shared" si="43"/>
+        <v>1</v>
+      </c>
+      <c r="N143" s="10">
         <f t="shared" si="46"/>
-        <v>1</v>
-      </c>
-      <c r="N143" s="10">
+        <v>0</v>
+      </c>
+      <c r="O143" s="10">
         <f t="shared" si="47"/>
-        <v>0</v>
-      </c>
-      <c r="O143" s="10">
-        <f t="shared" si="48"/>
         <v>0.5</v>
       </c>
     </row>
@@ -7982,15 +7979,15 @@
         <v>3</v>
       </c>
       <c r="M144" s="10">
+        <f t="shared" si="43"/>
+        <v>1</v>
+      </c>
+      <c r="N144" s="10">
         <f t="shared" si="46"/>
-        <v>1</v>
-      </c>
-      <c r="N144" s="10">
+        <v>0</v>
+      </c>
+      <c r="O144" s="10">
         <f t="shared" si="47"/>
-        <v>0</v>
-      </c>
-      <c r="O144" s="10">
-        <f t="shared" si="48"/>
         <v>0.5</v>
       </c>
     </row>
@@ -8032,14 +8029,15 @@
         <v>0</v>
       </c>
       <c r="M145" s="10">
+        <f t="shared" si="43"/>
         <v>0.5</v>
       </c>
       <c r="N145" s="10">
-        <f t="shared" ref="N145:N151" si="49">K145/(I145-L145)</f>
+        <f t="shared" ref="N145:N151" si="48">K145/(I145-L145)</f>
         <v>0.5</v>
       </c>
       <c r="O145" s="10">
-        <f t="shared" ref="O145:O151" si="50">I145/H145</f>
+        <f t="shared" ref="O145:O151" si="49">I145/H145</f>
         <v>0.5</v>
       </c>
     </row>
@@ -8081,14 +8079,15 @@
         <v>2</v>
       </c>
       <c r="M146" s="10">
+        <f t="shared" si="43"/>
         <v>1</v>
       </c>
       <c r="N146" s="10">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+      <c r="O146" s="10">
         <f t="shared" si="49"/>
-        <v>0</v>
-      </c>
-      <c r="O146" s="10">
-        <f t="shared" si="50"/>
         <v>0.5</v>
       </c>
     </row>
@@ -8130,14 +8129,15 @@
         <v>2</v>
       </c>
       <c r="M147" s="10">
+        <f t="shared" si="43"/>
         <v>1</v>
       </c>
       <c r="N147" s="10">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+      <c r="O147" s="10">
         <f t="shared" si="49"/>
-        <v>0</v>
-      </c>
-      <c r="O147" s="10">
-        <f t="shared" si="50"/>
         <v>0.5</v>
       </c>
     </row>
@@ -8179,14 +8179,15 @@
         <v>2</v>
       </c>
       <c r="M148" s="10">
+        <f t="shared" si="43"/>
         <v>1</v>
       </c>
       <c r="N148" s="10">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+      <c r="O148" s="10">
         <f t="shared" si="49"/>
-        <v>0</v>
-      </c>
-      <c r="O148" s="10">
-        <f t="shared" si="50"/>
         <v>0.5</v>
       </c>
     </row>
@@ -8228,14 +8229,15 @@
         <v>0</v>
       </c>
       <c r="M149" s="10">
+        <f t="shared" si="43"/>
         <v>1</v>
       </c>
       <c r="N149" s="10">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+      <c r="O149" s="10">
         <f t="shared" si="49"/>
-        <v>0</v>
-      </c>
-      <c r="O149" s="10">
-        <f t="shared" si="50"/>
         <v>0.5</v>
       </c>
     </row>
@@ -8277,14 +8279,15 @@
         <v>0</v>
       </c>
       <c r="M150" s="10">
+        <f t="shared" si="43"/>
         <v>0.75</v>
       </c>
       <c r="N150" s="10">
+        <f t="shared" si="48"/>
+        <v>0.25</v>
+      </c>
+      <c r="O150" s="10">
         <f t="shared" si="49"/>
-        <v>0.25</v>
-      </c>
-      <c r="O150" s="10">
-        <f t="shared" si="50"/>
         <v>0.5</v>
       </c>
     </row>
@@ -8326,15 +8329,366 @@
         <v>0</v>
       </c>
       <c r="M151" s="10">
+        <f t="shared" si="43"/>
         <v>1</v>
       </c>
       <c r="N151" s="10">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+      <c r="O151" s="10">
         <f t="shared" si="49"/>
-        <v>0</v>
-      </c>
-      <c r="O151" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A152" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B152" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C152" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D152" s="9">
+        <v>11</v>
+      </c>
+      <c r="E152" s="9">
+        <v>3</v>
+      </c>
+      <c r="F152" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G152" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="H152" s="5">
+        <v>10</v>
+      </c>
+      <c r="I152" s="5">
+        <v>5</v>
+      </c>
+      <c r="J152" s="5">
+        <v>2</v>
+      </c>
+      <c r="K152" s="5">
+        <v>2</v>
+      </c>
+      <c r="L152" s="5">
+        <v>1</v>
+      </c>
+      <c r="M152" s="10">
+        <f t="shared" si="43"/>
+        <v>0.5</v>
+      </c>
+      <c r="N152" s="10">
+        <f t="shared" ref="N152:N158" si="50">K152/(I152-L152)</f>
+        <v>0.5</v>
+      </c>
+      <c r="O152" s="10">
+        <f t="shared" ref="O152:O158" si="51">I152/H152</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A153" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B153" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C153" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D153" s="9">
+        <v>11</v>
+      </c>
+      <c r="E153" s="9">
+        <v>3</v>
+      </c>
+      <c r="F153" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G153" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H153" s="5">
+        <v>6</v>
+      </c>
+      <c r="I153" s="5">
+        <v>4</v>
+      </c>
+      <c r="J153" s="5">
+        <v>1</v>
+      </c>
+      <c r="K153" s="5">
+        <v>0</v>
+      </c>
+      <c r="L153" s="5">
+        <v>3</v>
+      </c>
+      <c r="M153" s="10">
+        <f t="shared" si="43"/>
+        <v>1</v>
+      </c>
+      <c r="N153" s="10">
         <f t="shared" si="50"/>
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="O153" s="10">
+        <f t="shared" si="51"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A154" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B154" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C154" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D154" s="9">
+        <v>11</v>
+      </c>
+      <c r="E154" s="9">
+        <v>3</v>
+      </c>
+      <c r="F154" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G154" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H154" s="5">
+        <v>6</v>
+      </c>
+      <c r="I154" s="5">
+        <v>4</v>
+      </c>
+      <c r="J154" s="5">
+        <v>1</v>
+      </c>
+      <c r="K154" s="5">
+        <v>0</v>
+      </c>
+      <c r="L154" s="5">
+        <v>3</v>
+      </c>
+      <c r="M154" s="10">
+        <f t="shared" si="43"/>
+        <v>1</v>
+      </c>
+      <c r="N154" s="10">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="O154" s="10">
+        <f t="shared" si="51"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A155" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B155" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C155" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D155" s="9">
+        <v>11</v>
+      </c>
+      <c r="E155" s="9">
+        <v>3</v>
+      </c>
+      <c r="F155" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G155" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H155" s="5">
+        <v>6</v>
+      </c>
+      <c r="I155" s="5">
+        <v>4</v>
+      </c>
+      <c r="J155" s="5">
+        <v>1</v>
+      </c>
+      <c r="K155" s="5">
+        <v>0</v>
+      </c>
+      <c r="L155" s="5">
+        <v>3</v>
+      </c>
+      <c r="M155" s="10">
+        <f t="shared" si="43"/>
+        <v>1</v>
+      </c>
+      <c r="N155" s="10">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="O155" s="10">
+        <f t="shared" si="51"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A156" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B156" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C156" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D156" s="9">
+        <v>11</v>
+      </c>
+      <c r="E156" s="9">
+        <v>3</v>
+      </c>
+      <c r="F156" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G156" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H156" s="5">
+        <v>6</v>
+      </c>
+      <c r="I156" s="5">
+        <v>4</v>
+      </c>
+      <c r="J156" s="5">
+        <v>3</v>
+      </c>
+      <c r="K156" s="5">
+        <v>0</v>
+      </c>
+      <c r="L156" s="5">
+        <v>1</v>
+      </c>
+      <c r="M156" s="10">
+        <f t="shared" si="43"/>
+        <v>1</v>
+      </c>
+      <c r="N156" s="10">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="O156" s="10">
+        <f t="shared" si="51"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A157" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B157" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C157" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D157" s="9">
+        <v>11</v>
+      </c>
+      <c r="E157" s="9">
+        <v>3</v>
+      </c>
+      <c r="F157" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G157" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H157" s="5">
+        <v>6</v>
+      </c>
+      <c r="I157" s="5">
+        <v>4</v>
+      </c>
+      <c r="J157" s="5">
+        <v>3</v>
+      </c>
+      <c r="K157" s="5">
+        <v>0</v>
+      </c>
+      <c r="L157" s="5">
+        <v>1</v>
+      </c>
+      <c r="M157" s="10">
+        <f t="shared" si="43"/>
+        <v>1</v>
+      </c>
+      <c r="N157" s="10">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="O157" s="10">
+        <f t="shared" si="51"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A158" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B158" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C158" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D158" s="9">
+        <v>11</v>
+      </c>
+      <c r="E158" s="9">
+        <v>3</v>
+      </c>
+      <c r="F158" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G158" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H158" s="5">
+        <v>6</v>
+      </c>
+      <c r="I158" s="5">
+        <v>5</v>
+      </c>
+      <c r="J158" s="5">
+        <v>5</v>
+      </c>
+      <c r="K158" s="5">
+        <v>0</v>
+      </c>
+      <c r="L158" s="5">
+        <v>0</v>
+      </c>
+      <c r="M158" s="10">
+        <f t="shared" si="43"/>
+        <v>1</v>
+      </c>
+      <c r="N158" s="10">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="O158" s="10">
+        <f t="shared" si="51"/>
+        <v>0.83333333333333337</v>
       </c>
     </row>
   </sheetData>
@@ -8346,10 +8700,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C53DFA-81F7-47CF-9345-E8C8EF0158AC}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:L568"/>
+  <dimension ref="A1:L598"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D549" workbookViewId="0">
-      <selection sqref="A1:J568"/>
+    <sheetView tabSelected="1" topLeftCell="A579" workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:J598"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25647,7 +26001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="541" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="541" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A541" s="9" t="s">
         <v>37</v>
       </c>
@@ -25679,7 +26033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="542" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="542" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A542" s="9" t="s">
         <v>37</v>
       </c>
@@ -25711,7 +26065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="543" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="543" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A543" s="9" t="s">
         <v>37</v>
       </c>
@@ -25743,7 +26097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="544" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A544" s="9" t="s">
         <v>37</v>
       </c>
@@ -25775,7 +26129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="545" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="545" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A545" s="9" t="s">
         <v>37</v>
       </c>
@@ -25807,7 +26161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="546" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="546" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A546" s="9" t="s">
         <v>37</v>
       </c>
@@ -25839,7 +26193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="547" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="547" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A547" s="9" t="s">
         <v>37</v>
       </c>
@@ -25871,7 +26225,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="548" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="548" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A548" s="9" t="s">
         <v>37</v>
       </c>
@@ -25903,7 +26257,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="549" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="549" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A549" s="9" t="s">
         <v>37</v>
       </c>
@@ -25935,7 +26289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="550" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="550" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A550" s="9" t="s">
         <v>37</v>
       </c>
@@ -25967,7 +26321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="551" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="551" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A551" s="9" t="s">
         <v>37</v>
       </c>
@@ -25999,7 +26353,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="552" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="552" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A552" s="9" t="s">
         <v>37</v>
       </c>
@@ -26031,7 +26385,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="553" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="553" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A553" s="9" t="s">
         <v>37</v>
       </c>
@@ -26063,7 +26417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="554" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="554" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A554" s="9" t="s">
         <v>37</v>
       </c>
@@ -26095,7 +26449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="555" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="555" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A555" s="9" t="s">
         <v>37</v>
       </c>
@@ -26127,7 +26481,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="556" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="556" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A556" s="9" t="s">
         <v>37</v>
       </c>
@@ -26159,7 +26513,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="557" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="557" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A557" s="9" t="s">
         <v>37</v>
       </c>
@@ -26191,7 +26545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="558" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="558" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A558" s="9" t="s">
         <v>37</v>
       </c>
@@ -26223,7 +26577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="559" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="559" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A559" s="9" t="s">
         <v>37</v>
       </c>
@@ -26242,7 +26596,7 @@
       <c r="F559" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G559" s="12" t="s">
+      <c r="G559" s="7" t="s">
         <v>47</v>
       </c>
       <c r="H559" s="9" t="s">
@@ -26255,7 +26609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="560" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="560" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A560" s="9" t="s">
         <v>37</v>
       </c>
@@ -26274,7 +26628,7 @@
       <c r="F560" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G560" s="12" t="s">
+      <c r="G560" s="7" t="s">
         <v>47</v>
       </c>
       <c r="H560" s="9" t="s">
@@ -26287,7 +26641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="561" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="561" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A561" s="9" t="s">
         <v>37</v>
       </c>
@@ -26306,7 +26660,7 @@
       <c r="F561" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G561" s="12" t="s">
+      <c r="G561" s="7" t="s">
         <v>47</v>
       </c>
       <c r="H561" s="9" t="s">
@@ -26319,7 +26673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="562" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="562" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A562" s="9" t="s">
         <v>37</v>
       </c>
@@ -26338,7 +26692,7 @@
       <c r="F562" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G562" s="12" t="s">
+      <c r="G562" s="7" t="s">
         <v>47</v>
       </c>
       <c r="H562" s="9" t="s">
@@ -26351,7 +26705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="563" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="563" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A563" s="9" t="s">
         <v>37</v>
       </c>
@@ -26370,7 +26724,7 @@
       <c r="F563" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G563" s="12" t="s">
+      <c r="G563" s="7" t="s">
         <v>49</v>
       </c>
       <c r="H563" s="9" t="s">
@@ -26383,7 +26737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="564" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="564" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A564" s="9" t="s">
         <v>37</v>
       </c>
@@ -26402,7 +26756,7 @@
       <c r="F564" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G564" s="12" t="s">
+      <c r="G564" s="7" t="s">
         <v>49</v>
       </c>
       <c r="H564" s="9" t="s">
@@ -26415,7 +26769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="565" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="565" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A565" s="9" t="s">
         <v>37</v>
       </c>
@@ -26434,7 +26788,7 @@
       <c r="F565" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G565" s="12" t="s">
+      <c r="G565" s="7" t="s">
         <v>49</v>
       </c>
       <c r="H565" s="9" t="s">
@@ -26447,7 +26801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="566" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="566" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A566" s="9" t="s">
         <v>37</v>
       </c>
@@ -26466,7 +26820,7 @@
       <c r="F566" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G566" s="12" t="s">
+      <c r="G566" s="7" t="s">
         <v>49</v>
       </c>
       <c r="H566" s="9" t="s">
@@ -26479,7 +26833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="567" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="567" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A567" s="9" t="s">
         <v>37</v>
       </c>
@@ -26498,7 +26852,7 @@
       <c r="F567" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G567" s="12" t="s">
+      <c r="G567" s="7" t="s">
         <v>53</v>
       </c>
       <c r="H567" s="9" t="s">
@@ -26511,7 +26865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="568" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="568" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A568" s="9" t="s">
         <v>37</v>
       </c>
@@ -26530,7 +26884,7 @@
       <c r="F568" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G568" s="12" t="s">
+      <c r="G568" s="7" t="s">
         <v>51</v>
       </c>
       <c r="H568" s="9" t="s">
@@ -26543,16 +26897,976 @@
         <v>1</v>
       </c>
     </row>
+    <row r="569" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A569" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B569" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C569" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D569" s="9">
+        <v>11</v>
+      </c>
+      <c r="E569" s="9">
+        <v>3</v>
+      </c>
+      <c r="F569" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G569" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H569" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I569" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J569" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="570" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A570" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B570" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C570" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D570" s="9">
+        <v>11</v>
+      </c>
+      <c r="E570" s="9">
+        <v>3</v>
+      </c>
+      <c r="F570" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G570" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H570" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I570" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J570" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="571" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A571" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B571" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C571" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D571" s="9">
+        <v>11</v>
+      </c>
+      <c r="E571" s="9">
+        <v>3</v>
+      </c>
+      <c r="F571" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G571" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H571" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I571" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J571" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="572" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A572" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B572" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C572" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D572" s="9">
+        <v>11</v>
+      </c>
+      <c r="E572" s="9">
+        <v>3</v>
+      </c>
+      <c r="F572" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G572" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H572" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I572" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J572" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="573" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A573" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B573" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C573" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D573" s="9">
+        <v>11</v>
+      </c>
+      <c r="E573" s="9">
+        <v>3</v>
+      </c>
+      <c r="F573" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G573" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H573" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I573" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="J573" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="574" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A574" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B574" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C574" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D574" s="9">
+        <v>11</v>
+      </c>
+      <c r="E574" s="9">
+        <v>3</v>
+      </c>
+      <c r="F574" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G574" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H574" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I574" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J574" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="575" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A575" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B575" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C575" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D575" s="9">
+        <v>11</v>
+      </c>
+      <c r="E575" s="9">
+        <v>3</v>
+      </c>
+      <c r="F575" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G575" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H575" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I575" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J575" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="576" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A576" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B576" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C576" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D576" s="9">
+        <v>11</v>
+      </c>
+      <c r="E576" s="9">
+        <v>3</v>
+      </c>
+      <c r="F576" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G576" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H576" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I576" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J576" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="577" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A577" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B577" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C577" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D577" s="9">
+        <v>11</v>
+      </c>
+      <c r="E577" s="9">
+        <v>3</v>
+      </c>
+      <c r="F577" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G577" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H577" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I577" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J577" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="578" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A578" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B578" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C578" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D578" s="9">
+        <v>11</v>
+      </c>
+      <c r="E578" s="9">
+        <v>3</v>
+      </c>
+      <c r="F578" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G578" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H578" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I578" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J578" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="579" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A579" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B579" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C579" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D579" s="9">
+        <v>11</v>
+      </c>
+      <c r="E579" s="9">
+        <v>3</v>
+      </c>
+      <c r="F579" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G579" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H579" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I579" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J579" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="580" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A580" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B580" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C580" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D580" s="9">
+        <v>11</v>
+      </c>
+      <c r="E580" s="9">
+        <v>3</v>
+      </c>
+      <c r="F580" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G580" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H580" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I580" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J580" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="581" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A581" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B581" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C581" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D581" s="9">
+        <v>11</v>
+      </c>
+      <c r="E581" s="9">
+        <v>3</v>
+      </c>
+      <c r="F581" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G581" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H581" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I581" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J581" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="582" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A582" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B582" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C582" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D582" s="9">
+        <v>11</v>
+      </c>
+      <c r="E582" s="9">
+        <v>3</v>
+      </c>
+      <c r="F582" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G582" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H582" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I582" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J582" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="583" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A583" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B583" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C583" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D583" s="9">
+        <v>11</v>
+      </c>
+      <c r="E583" s="9">
+        <v>3</v>
+      </c>
+      <c r="F583" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G583" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H583" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I583" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J583" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="584" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A584" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B584" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C584" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D584" s="9">
+        <v>11</v>
+      </c>
+      <c r="E584" s="9">
+        <v>3</v>
+      </c>
+      <c r="F584" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G584" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H584" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I584" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J584" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="585" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A585" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B585" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C585" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D585" s="9">
+        <v>11</v>
+      </c>
+      <c r="E585" s="9">
+        <v>3</v>
+      </c>
+      <c r="F585" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G585" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H585" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I585" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J585" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="586" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A586" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B586" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C586" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D586" s="9">
+        <v>11</v>
+      </c>
+      <c r="E586" s="9">
+        <v>3</v>
+      </c>
+      <c r="F586" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G586" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H586" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I586" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J586" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="587" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A587" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B587" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C587" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D587" s="9">
+        <v>11</v>
+      </c>
+      <c r="E587" s="9">
+        <v>3</v>
+      </c>
+      <c r="F587" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G587" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H587" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I587" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J587" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="588" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A588" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B588" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C588" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D588" s="9">
+        <v>11</v>
+      </c>
+      <c r="E588" s="9">
+        <v>3</v>
+      </c>
+      <c r="F588" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G588" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H588" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I588" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J588" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="589" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A589" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B589" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C589" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D589" s="9">
+        <v>11</v>
+      </c>
+      <c r="E589" s="9">
+        <v>3</v>
+      </c>
+      <c r="F589" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G589" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H589" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I589" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J589" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="590" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A590" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B590" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C590" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D590" s="9">
+        <v>11</v>
+      </c>
+      <c r="E590" s="9">
+        <v>3</v>
+      </c>
+      <c r="F590" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G590" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H590" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I590" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="J590" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="591" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A591" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B591" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C591" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D591" s="9">
+        <v>11</v>
+      </c>
+      <c r="E591" s="9">
+        <v>3</v>
+      </c>
+      <c r="F591" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G591" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H591" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I591" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="J591" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="592" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A592" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B592" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C592" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D592" s="9">
+        <v>11</v>
+      </c>
+      <c r="E592" s="9">
+        <v>3</v>
+      </c>
+      <c r="F592" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G592" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H592" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I592" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="J592" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="593" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A593" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B593" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C593" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D593" s="9">
+        <v>11</v>
+      </c>
+      <c r="E593" s="9">
+        <v>3</v>
+      </c>
+      <c r="F593" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G593" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H593" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I593" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="J593" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="594" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A594" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B594" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C594" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D594" s="9">
+        <v>11</v>
+      </c>
+      <c r="E594" s="9">
+        <v>3</v>
+      </c>
+      <c r="F594" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G594" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="H594" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I594" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J594" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="595" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A595" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B595" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C595" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D595" s="9">
+        <v>11</v>
+      </c>
+      <c r="E595" s="9">
+        <v>3</v>
+      </c>
+      <c r="F595" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G595" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H595" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I595" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J595" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="596" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A596" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B596" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C596" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D596" s="9">
+        <v>11</v>
+      </c>
+      <c r="E596" s="9">
+        <v>3</v>
+      </c>
+      <c r="F596" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G596" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H596" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I596" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J596" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="597" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A597" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B597" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C597" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D597" s="9">
+        <v>11</v>
+      </c>
+      <c r="E597" s="9">
+        <v>3</v>
+      </c>
+      <c r="F597" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G597" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H597" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I597" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J597" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="598" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A598" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B598" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C598" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D598" s="9">
+        <v>11</v>
+      </c>
+      <c r="E598" s="9">
+        <v>3</v>
+      </c>
+      <c r="F598" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G598" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H598" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I598" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="J598" s="9">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J568" xr:uid="{49C53DFA-81F7-47CF-9345-E8C8EF0158AC}">
-    <filterColumn colId="3">
+  <autoFilter ref="A1:J598" xr:uid="{49C53DFA-81F7-47CF-9345-E8C8EF0158AC}">
+    <filterColumn colId="2">
       <filters>
-        <filter val="11"/>
+        <filter val="November"/>
       </filters>
     </filterColumn>
     <filterColumn colId="4">
       <filters>
-        <filter val="2"/>
+        <filter val="3"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>